<commit_message>
Added openpyxl example data and code.
</commit_message>
<xml_diff>
--- a/data/xlsx/observationsummaries.xlsx
+++ b/data/xlsx/observationsummaries.xlsx
@@ -244,14 +244,14 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.88"/>

</xml_diff>